<commit_message>
commit orden de datos en index2
</commit_message>
<xml_diff>
--- a/Entregables.xlsx
+++ b/Entregables.xlsx
@@ -375,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +385,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +709,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +753,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -775,7 +776,7 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -798,7 +799,7 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -821,7 +822,7 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -844,7 +845,7 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -867,7 +868,7 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -890,7 +891,7 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -913,7 +914,7 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -936,7 +937,7 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -959,7 +960,7 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -982,7 +983,7 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1005,7 +1006,7 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1028,7 +1029,7 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1051,7 +1052,7 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1074,7 +1075,7 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1097,7 +1098,7 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1120,7 +1121,7 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1143,7 +1144,7 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1166,7 +1167,7 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1189,7 +1190,7 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1212,7 +1213,7 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1235,7 +1236,7 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1258,7 +1259,7 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1281,7 +1282,7 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1304,7 +1305,7 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1327,7 +1328,7 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1350,7 +1351,7 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1373,7 +1374,7 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="5">
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1396,7 +1397,7 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1419,7 +1420,7 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="5">
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1442,7 +1443,7 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="5">
         <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1465,7 +1466,7 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="5">
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1488,7 +1489,7 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="5">
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1511,7 +1512,7 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="5">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1534,7 +1535,7 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="5">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">

</xml_diff>